<commit_message>
Audiout: Improvements to input stage
</commit_message>
<xml_diff>
--- a/modules/Audiout/Audiout-BOM.xlsx
+++ b/modules/Audiout/Audiout-BOM.xlsx
@@ -1,38 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\Audiout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Audiout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FBA781-ED90-4A7D-BD34-B2CBAF663FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BE8C3E68-7684-44A0-8FF0-1CB2AC71C51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1230" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Audiout-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="183">
   <si>
     <t>Ref</t>
   </si>
@@ -148,25 +136,46 @@
     <t>C9 C10</t>
   </si>
   <si>
-    <t>470N</t>
-  </si>
-  <si>
-    <t>Capacitor - Film</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/datasheet/2/212/1/KEM_F3101_R82-1103738.pdf</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>R82DC3470SH60J</t>
-  </si>
-  <si>
-    <t>80-R82DC3470SH60J</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/?qs=Jv4FAWB%252B0HZ72wFOzKdj%2Fw%3D%3D</t>
+    <t>NPE</t>
+  </si>
+  <si>
+    <t>Capacitor - Non-polarized Electrolytic</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/315/ABA0000C1053-947510.pdf</t>
+  </si>
+  <si>
+    <t>ECE-A1EN100UI</t>
+  </si>
+  <si>
+    <t>667-ECE-A1EN100UI</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1EN100UI?qs=0h1gzos03f36mGOUyzNXaA%3D%3D</t>
+  </si>
+  <si>
+    <t>C11 C12</t>
+  </si>
+  <si>
+    <t>47P</t>
+  </si>
+  <si>
+    <t>Capacitor - Ceramic</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/427/VISH_S_A0012659393_1-2572337.pdf</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>K470K15C0GH53L2</t>
+  </si>
+  <si>
+    <t>594-K470K15C0GH53L2</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Vishay-BC-Components/K470K15C0GH53L2?qs=vmM6vcLFxxH%252BnUnXm2ihfA%3D%3D</t>
   </si>
   <si>
     <t>C15</t>
@@ -178,6 +187,21 @@
     <t>Capacitor - Electrolytic</t>
   </si>
   <si>
+    <t>https://www.mouser.ca/datasheet/2/977/e_YXJ-1601195.pdf</t>
+  </si>
+  <si>
+    <t>Rubycon</t>
+  </si>
+  <si>
+    <t>50YXJ1M5X11</t>
+  </si>
+  <si>
+    <t>232-50YXJ1M5X11</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Rubycon/50YXJ1M5X11?qs=T3oQrply3y9AG9vJ4bKZNQ%3D%3D</t>
+  </si>
+  <si>
     <t>C16 C17</t>
   </si>
   <si>
@@ -310,40 +334,94 @@
     <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61201621621?qs=ZtY9WdtwX55qFf4n3EFuaA%3D%3D</t>
   </si>
   <si>
-    <t>R1 R2 R3 R4 R19 R20</t>
+    <t>R1 R2</t>
+  </si>
+  <si>
+    <t>150K</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/447/Yageo_LR_MFR_1-1714151.pdf</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>MFR-12FTF52-150K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-150K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-150K?qs=oAGoVhmvjhyn6tjndOraRA%3D%3D</t>
+  </si>
+  <si>
+    <t>R3 R4</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>MFR-12FTF52-47K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-47K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FTF52-47K?qs=oAGoVhmvjhylO%2Fy0ChGYrw%3D%3D</t>
+  </si>
+  <si>
+    <t>R5 R6 R7 R8 R29 R30 R31 R32</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>MFR-12FRF52-10K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FRF5210K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-12FRF52-10K?qs=19cKSROHwrBLAZVjkXsohw%3D%3D</t>
+  </si>
+  <si>
+    <t>R9 R10</t>
+  </si>
+  <si>
+    <t>43K2</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/datasheet/2/427/cmfmil-1762972.pdf</t>
+  </si>
+  <si>
+    <t>Vishay / Dale</t>
+  </si>
+  <si>
+    <t>RN55D4322FRE6</t>
+  </si>
+  <si>
+    <t>71-RN55D-F-43.2K/R</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Vishay-Dale/RN55D4322FRE6?qs=uspOzq2yv%2FMqqeE%2Fvm%252BOVQ%3D%3D</t>
+  </si>
+  <si>
+    <t>R11 R12 R19 R20</t>
   </si>
   <si>
     <t>100K</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R5 R6 R7 R8 R29 R30 R31 R32</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R9 R10</t>
-  </si>
-  <si>
-    <t>43K2</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/datasheet/2/427/cmfmil-1762972.pdf</t>
-  </si>
-  <si>
-    <t>Vishay / Dale</t>
-  </si>
-  <si>
-    <t>RN55D4322FRE6</t>
-  </si>
-  <si>
-    <t>71-RN55D-F-43.2K/R</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/Vishay-Dale/RN55D4322FRE6?qs=uspOzq2yv%2FMqqeE%2Fvm%252BOVQ%3D%3D</t>
+    <t>MFR-12FTF52-100K</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-100K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/603-MFR-12FTF52-100K</t>
   </si>
   <si>
     <t>R15 R16 R17 R18</t>
@@ -356,12 +434,6 @@
   </si>
   <si>
     <t>Output limiting</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/datasheet/2/447/Yageo_LR_MFR_1-1714151.pdf</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
   </si>
   <si>
     <t>MFR-25FTF52-100R</t>
@@ -502,7 +574,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1348,20 +1420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="4.59765625" customWidth="1"/>
+    <col min="2" max="5" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1369,13 +1441,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1426,7 +1498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1551,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E22" si="0">MAX(0,B3-C3-D3)</f>
+        <f t="shared" ref="E3:E25" si="0">MAX(0,B3-C3-D3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1510,21 +1582,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
         <v>38</v>
       </c>
       <c r="I4" t="s">
@@ -1534,84 +1606,99 @@
         <v>40</v>
       </c>
       <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
         <v>41</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
       </c>
       <c r="M4" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
         <v>43</v>
       </c>
-      <c r="O4" t="s">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>47</v>
       </c>
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="M6" t="s">
         <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1624,33 +1711,33 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
         <v>23</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
         <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="O7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1663,111 +1750,129 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O8" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>70</v>
-      </c>
-      <c r="R8" t="s">
         <v>71</v>
       </c>
-      <c r="S8" t="s">
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="T8">
-        <v>4031</v>
-      </c>
-      <c r="U8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>74</v>
-      </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" t="s">
         <v>75</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>77</v>
       </c>
-      <c r="K9" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>78</v>
-      </c>
-      <c r="M9" t="s">
-        <v>66</v>
       </c>
       <c r="N9" t="s">
         <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>68</v>
+        <v>80</v>
+      </c>
+      <c r="P9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R9" t="s">
+        <v>83</v>
+      </c>
+      <c r="S9" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9">
+        <v>4031</v>
+      </c>
+      <c r="U9" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>88</v>
+      </c>
+      <c r="J10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" t="s">
+        <v>90</v>
+      </c>
+      <c r="M10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1780,15 +1885,15 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1801,395 +1906,524 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="I12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" t="s">
-        <v>89</v>
-      </c>
-      <c r="L12">
-        <v>61201621621</v>
-      </c>
-      <c r="M12" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" t="s">
-        <v>90</v>
-      </c>
-      <c r="O12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>99</v>
+      </c>
+      <c r="J13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13">
+        <v>61201621621</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O13" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>106</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" t="s">
+        <v>110</v>
+      </c>
+      <c r="O14" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="L15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="M15" t="s">
         <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="O15" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" t="s">
         <v>106</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>107</v>
       </c>
-      <c r="I16" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>108</v>
       </c>
-      <c r="K16" t="s">
-        <v>109</v>
-      </c>
       <c r="L16" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="M16" t="s">
         <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="O16" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="J17" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K17" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="L17" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="M17" t="s">
         <v>25</v>
       </c>
       <c r="N17" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="O17" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="J18" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="L18" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="M18" t="s">
         <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="O18" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>136</v>
+      </c>
+      <c r="H19" t="s">
+        <v>137</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="J19" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="K19" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="L19" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="M19" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="N19" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="O19" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="I20" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="J20" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="K20" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="L20" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="M20" t="s">
         <v>25</v>
       </c>
       <c r="N20" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="O20" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="J21" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="K21" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L21" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="M21" t="s">
         <v>25</v>
       </c>
       <c r="N21" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="O21" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>130</v>
+      </c>
+      <c r="G22" t="s">
+        <v>152</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="J22" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="K22" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="L22" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="M22" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+      <c r="I23" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K23" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" t="s">
         <v>25</v>
       </c>
-      <c r="N22" t="s">
-        <v>150</v>
-      </c>
-      <c r="O22" t="s">
-        <v>151</v>
+      <c r="N23" t="s">
+        <v>165</v>
+      </c>
+      <c r="O23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>168</v>
+      </c>
+      <c r="I24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" t="s">
+        <v>162</v>
+      </c>
+      <c r="K24" t="s">
+        <v>163</v>
+      </c>
+      <c r="L24" t="s">
+        <v>170</v>
+      </c>
+      <c r="M24" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" t="s">
+        <v>171</v>
+      </c>
+      <c r="O24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J25" t="s">
+        <v>176</v>
+      </c>
+      <c r="K25" t="s">
+        <v>163</v>
+      </c>
+      <c r="L25" t="s">
+        <v>177</v>
+      </c>
+      <c r="M25" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" t="s">
+        <v>178</v>
+      </c>
+      <c r="O25" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E22">
+  <conditionalFormatting sqref="E2:E25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>